<commit_message>
elec calibration guaranteed dispatc
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bgdpbes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Ohio\OH-eps\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B831B-97A2-1F47-B0E7-C814EF427FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C28837-7C2F-4939-8A7C-AA6FB3D4C0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23000" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="1710" windowWidth="15585" windowHeight="14670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -153,15 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -503,54 +497,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="2">
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -568,19 +562,19 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1">
         <v>2015</v>
       </c>
       <c r="C1">
@@ -689,7 +683,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -697,147 +691,112 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>$B2</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:AK9" si="0">$B2</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="H2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ2">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -845,147 +804,112 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:R12" si="1">$B3</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ3">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -993,147 +917,112 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="W4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1141,147 +1030,112 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1289,147 +1143,112 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ6">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1437,147 +1256,112 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1585,147 +1369,112 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ8">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AK8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1733,147 +1482,112 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AJ9">
-        <f t="shared" ref="D9:AK14" si="2">$B9</f>
         <v>0</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1881,147 +1595,112 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ10">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2029,147 +1708,112 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2177,147 +1821,112 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2325,147 +1934,112 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>$B13</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2473,147 +2047,112 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>$B14</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2839,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>

</xml_diff>